<commit_message>
update process info comments
</commit_message>
<xml_diff>
--- a/LDPowerHarvesComputations.xlsx
+++ b/LDPowerHarvesComputations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Max HP</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>PV/heal</t>
+  </si>
+  <si>
+    <t>RCL need:</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -195,15 +198,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -212,6 +223,10 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +510,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,252 +522,264 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="9"/>
+      <c r="E2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>2000000</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f>C3/C4</f>
         <v>66666.666666666672</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>F6*C4*C9</f>
         <v>300</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>30</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f>F3/C14</f>
         <v>47.61904761904762</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="4" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>12</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>80</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>20</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f>_xlfn.CEILING.MATH(I3/C5)</f>
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>250</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f>MIN(50-F6,F6)</f>
         <v>20</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>MIN(50-I6,I6)</f>
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>50</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f>_xlfn.CEILING.MATH(F6/F7)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f>_xlfn.CEILING.MATH(I6/I7)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.5</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1500</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f>_xlfn.CEILING.MATH(F4/F6)</f>
         <v>3</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>F10</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <f>F6*C6+F7*C8</f>
         <v>2600</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f>I6*C7+I7*C8</f>
         <v>7500</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="9"/>
+      <c r="E13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="10">
+        <v>7</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="10">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1400</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>0.85</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f>C3/(C4*F6*F10)</f>
         <v>1111.1111111111111</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f>F10*F12+I12*I10</f>
         <v>30300</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <f>((C10-C20)*C15)/(MAX(F8,I8))</f>
         <v>330.55555555555554</v>
       </c>

</xml_diff>

<commit_message>
Comments added before coding
</commit_message>
<xml_diff>
--- a/LDPowerHarvesComputations.xlsx
+++ b/LDPowerHarvesComputations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Max HP</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>RCL need:</t>
+  </si>
+  <si>
+    <t>RCL capa:</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
@@ -213,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -223,10 +232,16 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L22"/>
+  <dimension ref="B2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,21 +536,21 @@
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
@@ -596,7 +611,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -617,7 +632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -638,8 +653,12 @@
         <f>MIN(50-I6,I6)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -660,8 +679,14 @@
         <f>_xlfn.CEILING.MATH(I6/I7)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -672,8 +697,14 @@
       <c r="F9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="12">
+        <v>300</v>
+      </c>
+      <c r="M9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
@@ -694,14 +725,26 @@
         <f>F10</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="12">
+        <v>550</v>
+      </c>
+      <c r="M10" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="12">
+        <v>800</v>
+      </c>
+      <c r="M11" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,46 +759,78 @@
         <f>I6*C7+I7*C8</f>
         <v>7500</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="L12" s="12">
+        <v>1300</v>
+      </c>
+      <c r="M12" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="10"/>
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>7</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="12">
+        <v>1800</v>
+      </c>
+      <c r="M13" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2">
         <v>1400</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="12">
+        <v>2300</v>
+      </c>
+      <c r="M14" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="7">
         <v>0.85</v>
       </c>
+      <c r="L15" s="12">
+        <v>5300</v>
+      </c>
+      <c r="M15" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="12">
+        <v>12900</v>
+      </c>
+      <c r="M16" s="12">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -785,7 +860,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>

</xml_diff>